<commit_message>
Add Overview with Data Description
</commit_message>
<xml_diff>
--- a/01_Data/HomeCredit_columns_description_formatted.xlsx
+++ b/01_Data/HomeCredit_columns_description_formatted.xlsx
@@ -9,7 +9,11 @@
   <sheets>
     <sheet name="HomeCredit_columns_description" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle2[#All]</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">HomeCredit_columns_description!$1:$1</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1814,39 +1818,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1942,13 +1913,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1963,20 +1927,60 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:E220" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:E220" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E220"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Table" dataDxfId="4"/>
-    <tableColumn id="3" name="Row" dataDxfId="3"/>
-    <tableColumn id="4" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" name="Special" dataDxfId="1"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Table" dataDxfId="3"/>
+    <tableColumn id="3" name="Row" dataDxfId="2"/>
+    <tableColumn id="4" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" name="Special" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2267,9 +2271,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5757,8 +5764,8 @@
       <c r="E220" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>